<commit_message>
increased privacy in sheets
</commit_message>
<xml_diff>
--- a/sheets/colic.xlsx
+++ b/sheets/colic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\OneDrive\Desktop\chaos\sigma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83A6EEB-099B-4646-BDB5-5ACB1239E891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A065F7A-6CA0-4A8F-A136-E89378D01A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterplan" sheetId="1" r:id="rId1"/>
@@ -31,51 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={F84E22E6-CD70-4533-9EFF-94F49C06BDC1}</author>
-    <author>tc={7F44340F-68A5-4369-802E-02824564DD12}</author>
-    <author>tc={3DC8C580-79B3-487D-BC23-955992DB1952}</author>
-    <author>tc={D10F7B7F-9F4D-433E-BB20-9AC7819829EA}</author>
-  </authors>
-  <commentList>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{F84E22E6-CD70-4533-9EFF-94F49C06BDC1}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    🎂 Rybicki</t>
-      </text>
-    </comment>
-    <comment ref="G7" authorId="1" shapeId="0" xr:uid="{7F44340F-68A5-4369-802E-02824564DD12}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    🎂 Olmes</t>
-      </text>
-    </comment>
-    <comment ref="G20" authorId="2" shapeId="0" xr:uid="{3DC8C580-79B3-487D-BC23-955992DB1952}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    🎂 Huber</t>
-      </text>
-    </comment>
-    <comment ref="Q49" authorId="3" shapeId="0" xr:uid="{D10F7B7F-9F4D-433E-BB20-9AC7819829EA}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    🎂 Koteski, Tienietilov</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1033,9 +988,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Nicola.Colic" id="{546AED49-75D9-4F2F-AE01-3C753031FA6E}" userId="S::Nicola.Colic@bbbaden.ch::9bb3231b-f16f-46b6-a871-3746f182172e" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1333,33 +1286,16 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G5" dT="2024-08-12T07:28:37.54" personId="{546AED49-75D9-4F2F-AE01-3C753031FA6E}" id="{F84E22E6-CD70-4533-9EFF-94F49C06BDC1}">
-    <text>🎂 Rybicki</text>
-  </threadedComment>
-  <threadedComment ref="G7" dT="2024-08-12T07:29:52.63" personId="{546AED49-75D9-4F2F-AE01-3C753031FA6E}" id="{7F44340F-68A5-4369-802E-02824564DD12}">
-    <text>🎂 Olmes</text>
-  </threadedComment>
-  <threadedComment ref="G20" dT="2024-08-12T07:32:05.69" personId="{546AED49-75D9-4F2F-AE01-3C753031FA6E}" id="{3DC8C580-79B3-487D-BC23-955992DB1952}">
-    <text>🎂 Huber</text>
-  </threadedComment>
-  <threadedComment ref="Q49" dT="2024-08-12T07:31:30.64" personId="{546AED49-75D9-4F2F-AE01-3C753031FA6E}" id="{D10F7B7F-9F4D-433E-BB20-9AC7819829EA}">
-    <text>🎂 Koteski, Tienietilov</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="3" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M60" sqref="M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -3543,7 +3479,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -3643,12 +3578,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f623eb36-e09d-4262-8e82-8bdef17c0a1d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12d55486-500d-4026-8344-9329d1f6ef49">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3853,20 +3790,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f623eb36-e09d-4262-8e82-8bdef17c0a1d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12d55486-500d-4026-8344-9329d1f6ef49">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EAD0523-541D-4D5E-8A8E-693E501F75DA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D9C7833-16CE-46EF-875D-321A76CB25C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f623eb36-e09d-4262-8e82-8bdef17c0a1d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="12d55486-500d-4026-8344-9329d1f6ef49"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3891,18 +3835,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D9C7833-16CE-46EF-875D-321A76CB25C1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EAD0523-541D-4D5E-8A8E-693E501F75DA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f623eb36-e09d-4262-8e82-8bdef17c0a1d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="12d55486-500d-4026-8344-9329d1f6ef49"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>